<commit_message>
Now reporting protocol position. Added presets.
</commit_message>
<xml_diff>
--- a/src_mcu/Serial_commands.xlsx
+++ b/src_mcu/Serial_commands.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\_GitHub_repo\project-TWT-jetting-grid\src_mcu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C8FD4C-5FFD-4354-9B99-A0C7F134649C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45A6084-AEEF-4AFA-9AFA-3AF28453D8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10470" yWindow="1185" windowWidth="15345" windowHeight="12600" xr2:uid="{770A8635-2E22-4927-94A5-DB55E37C9D0A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$C$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$D$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>id?</t>
   </si>
@@ -132,12 +132,6 @@
     <t>Load protocol preset: Walk over each single valve</t>
   </si>
   <si>
-    <t>Load protocol preset: Alternate 50/50 between even- and odd-numbered valves</t>
-  </si>
-  <si>
-    <t>Load protocol preset: Alternate 50/50 checkerboard pattern</t>
-  </si>
-  <si>
     <t>Play the protocol and automatically actuate valves over time</t>
   </si>
   <si>
@@ -195,6 +189,24 @@
 - protocol_pos (index starts at 1)
 - pres_#_mA
 - pres_#_bar</t>
+  </si>
+  <si>
+    <t>Additional reply</t>
+  </si>
+  <si>
+    <t>Current protocol position `pos`</t>
+  </si>
+  <si>
+    <t>Load protocol preset: Alternating checkerboard</t>
+  </si>
+  <si>
+    <t>Load protocol preset: Alternating even/odd valves</t>
+  </si>
+  <si>
+    <t>preset4</t>
+  </si>
+  <si>
+    <t>Load protocol preset: Walk over each manifold</t>
   </si>
 </sst>
 </file>
@@ -276,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -293,16 +305,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -622,218 +628,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7E2509-F29D-4A31-A0BD-5D684EC3EA3F}">
-  <dimension ref="B1:C30"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D30" sqref="B1:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.86328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="51.265625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.06640625" style="1"/>
+    <col min="4" max="4" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="B1" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="B1" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D3" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="2:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="57" x14ac:dyDescent="0.45">
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="2:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="B9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C9" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B12" s="7" t="s">
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B20" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B19" s="7" t="s">
+      <c r="C20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B20" s="7" t="s">
+      <c r="C21" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B22" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B21" s="7" t="s">
+      <c r="C22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B25" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B22" s="7" t="s">
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B28" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B24" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B25" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="9" t="s">
+    </row>
+    <row r="29" spans="2:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B26" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B27" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B28" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B29" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="C30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="92" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Major changes: streamlined presets mechanism & keeping track of protocol name
</commit_message>
<xml_diff>
--- a/src_mcu/Serial_commands.xlsx
+++ b/src_mcu/Serial_commands.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\_GitHub_repo\project-TWT-jetting-grid\src_mcu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1017075A-2837-44C8-979F-1B24E4CAC919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6261319E-B56C-4155-BC9A-FD463FFA238C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="2616" windowWidth="20928" windowHeight="14100" xr2:uid="{770A8635-2E22-4927-94A5-DB55E37C9D0A}"/>
+    <workbookView xWindow="5784" yWindow="4392" windowWidth="20928" windowHeight="14100" xr2:uid="{770A8635-2E22-4927-94A5-DB55E37C9D0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$D$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$D$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>id?</t>
   </si>
@@ -144,9 +144,6 @@
     <t>preset3</t>
   </si>
   <si>
-    <t>Report current line buffer contents</t>
-  </si>
-  <si>
     <t>Trigger a halt</t>
   </si>
   <si>
@@ -157,11 +154,6 @@
   </si>
   <si>
     <t>TWT Jetting Grid, Arduino serial commands</t>
-  </si>
-  <si>
-    <t>Report current protocol info, newline delimited:
-- protocol name
-- N_lines</t>
   </si>
   <si>
     <t>Report readings, tab delimited:
@@ -173,9 +165,6 @@
     <t>Additional reply</t>
   </si>
   <si>
-    <t>Current protocol position `pos`</t>
-  </si>
-  <si>
     <t>Load protocol preset: Alternating checkerboard</t>
   </si>
   <si>
@@ -207,6 +196,23 @@
   </si>
   <si>
     <t>Load protocol preset: Walk over all manifolds</t>
+  </si>
+  <si>
+    <t>Report current protocol info, tab delimited:
+- protocol name
+- N_lines</t>
+  </si>
+  <si>
+    <t>p?</t>
+  </si>
+  <si>
+    <t>{pos}</t>
+  </si>
+  <si>
+    <t>Pretty print the full protocol program</t>
+  </si>
+  <si>
+    <t>Pretty print the current line buffer contents</t>
   </si>
 </sst>
 </file>
@@ -631,10 +637,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:D30"/>
+  <dimension ref="B1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,7 +654,7 @@
   <sheetData>
     <row r="1" spans="2:4" ht="18" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -659,7 +665,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -684,15 +690,15 @@
         <v>9</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -700,7 +706,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
@@ -731,10 +737,10 @@
         <v>24</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -742,10 +748,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -753,10 +759,10 @@
         <v>6</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -764,10 +770,10 @@
         <v>7</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -775,10 +781,10 @@
         <v>8</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
@@ -786,7 +792,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D19" s="6"/>
     </row>
@@ -795,7 +801,7 @@
         <v>27</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D20" s="6"/>
     </row>
@@ -804,7 +810,7 @@
         <v>28</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D21" s="6"/>
     </row>
@@ -813,16 +819,16 @@
         <v>29</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D22" s="6"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D23" s="6"/>
     </row>
@@ -836,39 +842,47 @@
         <v>10</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B29" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="C29" s="7" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B31" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>32</v>
+      <c r="C31" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>